<commit_message>
Update Excel Spreadsheet for all database.xlsx
</commit_message>
<xml_diff>
--- a/Data/Excel Spreadsheet for all database.xlsx
+++ b/Data/Excel Spreadsheet for all database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakri\Documents\GitHub\Group3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CD333C-2AA6-41B0-AC53-100002B05CB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7417B5A4-FF80-4693-895A-7C603848D597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BE2676A-B838-423E-A028-24E9E443D268}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="688" firstSheet="1" activeTab="13" xr2:uid="{5BE2676A-B838-423E-A028-24E9E443D268}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="227">
   <si>
     <t>User</t>
   </si>
@@ -103,9 +103,6 @@
     <t>TraderEmail</t>
   </si>
   <si>
-    <t>TraderPaasword</t>
-  </si>
-  <si>
     <t>TraderAddress</t>
   </si>
   <si>
@@ -193,12 +190,6 @@
     <t>ProductStock</t>
   </si>
   <si>
-    <t>AlleryInfromation</t>
-  </si>
-  <si>
-    <t>ProductQuantity</t>
-  </si>
-  <si>
     <t>ProductImage</t>
   </si>
   <si>
@@ -284,13 +275,475 @@
   </si>
   <si>
     <t>CollectionDay</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>Bakery</t>
+  </si>
+  <si>
+    <t>Aura</t>
+  </si>
+  <si>
+    <t>Blue Chesire</t>
+  </si>
+  <si>
+    <t>Dolce Latte</t>
+  </si>
+  <si>
+    <t>Labard Blue</t>
+  </si>
+  <si>
+    <t>Feta</t>
+  </si>
+  <si>
+    <t>Gruyere</t>
+  </si>
+  <si>
+    <t>Mojarella</t>
+  </si>
+  <si>
+    <t>Quesco Fresco</t>
+  </si>
+  <si>
+    <t>Cojita</t>
+  </si>
+  <si>
+    <t>Emmental</t>
+  </si>
+  <si>
+    <t>Guana Popdara</t>
+  </si>
+  <si>
+    <t>Parmesan</t>
+  </si>
+  <si>
+    <t>Lactose Intolerant</t>
+  </si>
+  <si>
+    <t>Cheddar</t>
+  </si>
+  <si>
+    <t>Comte</t>
+  </si>
+  <si>
+    <t>Gouda</t>
+  </si>
+  <si>
+    <t>Tallejio</t>
+  </si>
+  <si>
+    <t>AlleryInformation</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Pandey</t>
+  </si>
+  <si>
+    <t>rpandey@gmail.com</t>
+  </si>
+  <si>
+    <t>Kathmandu</t>
+  </si>
+  <si>
+    <t>Sakriya</t>
+  </si>
+  <si>
+    <t>Bajracharya</t>
+  </si>
+  <si>
+    <t>sakriya33@gmail.com</t>
+  </si>
+  <si>
+    <t>TraderPassword</t>
+  </si>
+  <si>
+    <t>Swastika</t>
+  </si>
+  <si>
+    <t>Adhikari</t>
+  </si>
+  <si>
+    <t>swasti@gmail.com</t>
+  </si>
+  <si>
+    <t>Sujan</t>
+  </si>
+  <si>
+    <t>Pariyar</t>
+  </si>
+  <si>
+    <t>spariyar@gmail.com</t>
+  </si>
+  <si>
+    <t>Prasanna</t>
+  </si>
+  <si>
+    <t>Shrestha</t>
+  </si>
+  <si>
+    <t>pshrestha@gmail.com</t>
+  </si>
+  <si>
+    <t>Utsav</t>
+  </si>
+  <si>
+    <t>Sapkota</t>
+  </si>
+  <si>
+    <t>usapkota@gmial.com</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>Bessemer</t>
+  </si>
+  <si>
+    <t>Alexander City</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Andalusia</t>
+  </si>
+  <si>
+    <t>Anniston</t>
+  </si>
+  <si>
+    <t>Chickasaw</t>
+  </si>
+  <si>
+    <t>Clanton</t>
+  </si>
+  <si>
+    <t>Athens</t>
+  </si>
+  <si>
+    <t>Atmore</t>
+  </si>
+  <si>
+    <t>arleengunder@gmail.com</t>
+  </si>
+  <si>
+    <t>mariannapgar@gmail.com</t>
+  </si>
+  <si>
+    <t>colleenestepp@gmail.com</t>
+  </si>
+  <si>
+    <t>michaelchaplin@gmail.com</t>
+  </si>
+  <si>
+    <t>geralynmunns@gmail.com</t>
+  </si>
+  <si>
+    <t>nellhong@gmail.com</t>
+  </si>
+  <si>
+    <t>charlsiesteigerwald@gmail.com</t>
+  </si>
+  <si>
+    <t>fernandahedden@gmail.com</t>
+  </si>
+  <si>
+    <t>wilbertauman@gmail.com</t>
+  </si>
+  <si>
+    <t>dorseycoit@gmail.com</t>
+  </si>
+  <si>
+    <t>Gunder</t>
+  </si>
+  <si>
+    <t>Arleen</t>
+  </si>
+  <si>
+    <t>Mariann</t>
+  </si>
+  <si>
+    <t>Apgar</t>
+  </si>
+  <si>
+    <t>Nell</t>
+  </si>
+  <si>
+    <t>Hong</t>
+  </si>
+  <si>
+    <t>Colleen</t>
+  </si>
+  <si>
+    <t>Estepp</t>
+  </si>
+  <si>
+    <t>Charlsie</t>
+  </si>
+  <si>
+    <t>Steigerwald</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
+  </si>
+  <si>
+    <t>Hedden</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Chaplin</t>
+  </si>
+  <si>
+    <t>Geralyn</t>
+  </si>
+  <si>
+    <t>Munns</t>
+  </si>
+  <si>
+    <t>Wilbert</t>
+  </si>
+  <si>
+    <t>Auman</t>
+  </si>
+  <si>
+    <t>Dorsey</t>
+  </si>
+  <si>
+    <t>Coit</t>
+  </si>
+  <si>
+    <t>Arleen123</t>
+  </si>
+  <si>
+    <t>Mariann234</t>
+  </si>
+  <si>
+    <t>Nell345</t>
+  </si>
+  <si>
+    <t>Colleen456</t>
+  </si>
+  <si>
+    <t>Charlsie567</t>
+  </si>
+  <si>
+    <t>Fernanda678</t>
+  </si>
+  <si>
+    <t>Michael789</t>
+  </si>
+  <si>
+    <t>Geralyn890</t>
+  </si>
+  <si>
+    <t>Wilbert098</t>
+  </si>
+  <si>
+    <t>Dorsey978</t>
+  </si>
+  <si>
+    <t>Hygienic Meat Shop</t>
+  </si>
+  <si>
+    <t>Naughty Pig Butchery &amp; Encased Meats</t>
+  </si>
+  <si>
+    <t>The Golden Grate</t>
+  </si>
+  <si>
+    <t>Praise cheeses!</t>
+  </si>
+  <si>
+    <t>Groomers Seafood.</t>
+  </si>
+  <si>
+    <t>River Thrive.</t>
+  </si>
+  <si>
+    <r>
+      <t>Deli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bros</t>
+    </r>
+  </si>
+  <si>
+    <t>The Yellow Submarine</t>
+  </si>
+  <si>
+    <t>Red Velvet Bakery</t>
+  </si>
+  <si>
+    <t>New Road</t>
+  </si>
+  <si>
+    <t>Queens Road</t>
+  </si>
+  <si>
+    <t>Alexander Road</t>
+  </si>
+  <si>
+    <t>Station Road</t>
+  </si>
+  <si>
+    <t>Green Lane</t>
+  </si>
+  <si>
+    <t>The Grove</t>
+  </si>
+  <si>
+    <t>Church Road</t>
+  </si>
+  <si>
+    <t>Queensway</t>
+  </si>
+  <si>
+    <t>Stanley Road</t>
+  </si>
+  <si>
+    <t>Chester Road</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Flat Bread</t>
+  </si>
+  <si>
+    <t>Bagel</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Muffin</t>
+  </si>
+  <si>
+    <t>Doughnut</t>
+  </si>
+  <si>
+    <t>Buns</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Pastries</t>
+  </si>
+  <si>
+    <t>Pita</t>
+  </si>
+  <si>
+    <t>CornBread</t>
+  </si>
+  <si>
+    <t>SodaBread</t>
+  </si>
+  <si>
+    <t>Crumpets</t>
+  </si>
+  <si>
+    <t>Tarts</t>
+  </si>
+  <si>
+    <t>Crackers</t>
+  </si>
+  <si>
+    <t>Wheat and Yeast Allergies</t>
+  </si>
+  <si>
+    <t>Anytime Cakes</t>
+  </si>
+  <si>
+    <t>Cheese is a dairy product, derived from milk and produced in a wide range of flavors, textures and forms by coagulation of the milk protein casein.</t>
+  </si>
+  <si>
+    <t>A bakery is an establishment that produces and sells flour-based food baked in an oven such as bread, cookies, cakes, pastries, and pies.</t>
+  </si>
+  <si>
+    <t>Birthday Cake</t>
+  </si>
+  <si>
+    <t>Black Forest</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Red Velvet</t>
+  </si>
+  <si>
+    <t>Peanut Cake</t>
+  </si>
+  <si>
+    <t>Coconut Choclate Cake</t>
+  </si>
+  <si>
+    <t>Strawberry Cake</t>
+  </si>
+  <si>
+    <t>Choclate Fruit Cake</t>
+  </si>
+  <si>
+    <t>Moose Fruit Cake</t>
+  </si>
+  <si>
+    <t>Chocolate Birthday Cake</t>
+  </si>
+  <si>
+    <t>Nuts Cake</t>
+  </si>
+  <si>
+    <t>Wallnut Ckae</t>
+  </si>
+  <si>
+    <t>Cherry Cake</t>
+  </si>
+  <si>
+    <t>Red Vanilla Cake</t>
+  </si>
+  <si>
+    <t>Butterscotch Cake</t>
+  </si>
+  <si>
+    <t>Vlentine Cake</t>
+  </si>
+  <si>
+    <t>Cake is a form of sweet food made from flour, sugar, and other ingredients, that is usually baked. In their oldest forms, cakes were modifications of bread</t>
+  </si>
+  <si>
+    <t>Wheat and Yeast Allergies, Lactose Intolerant, Eggs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +754,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,14 +791,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAAA82E-906A-4140-A365-83DC95A237A9}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -666,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -700,50 +1175,52 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBF54B2-6D09-4EC6-9D9F-49DC6D95A617}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>150001</v>
       </c>
@@ -769,15 +1246,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -809,24 +1286,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -856,21 +1333,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -887,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F329ED14-84C5-4A2A-A784-5736BC6EFAF3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,18 +1377,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -924,7 +1401,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,25 +1435,43 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10001</v>
       </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3">
+        <v>132456</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{647AEB61-F663-4A2F-B0BE-DF4703BD9F96}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F42D55-32F9-4B5C-B060-382E558DA586}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,31 +1503,133 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>200001</v>
       </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3">
+        <v>123456</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>200002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4">
+        <v>123456</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>200003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5">
+        <v>123456</v>
+      </c>
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>200004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6">
+        <v>123456</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>200005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7">
+        <v>123456</v>
+      </c>
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{76FF674B-DF1B-4597-9762-B457A2401787}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{CD7137DC-34FF-43D7-9A01-F77774486DE9}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{147F4E02-2906-4E51-8098-C7AFED7CCBC5}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{FABA20FF-08B0-49C4-9E82-C703C66588C7}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{8E76655F-BC31-4B3D-A745-20E5586B2798}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD787E46-28B6-42DB-B9B0-AF8A27F3208F}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,44 +1647,281 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>30001</v>
       </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="3">
+        <v>11818</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>30002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="3">
+        <v>12161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>30003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="3">
+        <v>16145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>30004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="3">
+        <v>22011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>30005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="3">
+        <v>24402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>30006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="3">
+        <v>25811</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>30007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="3">
+        <v>25955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>30008</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="3">
+        <v>28121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>30009</v>
+      </c>
+      <c r="B11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="3">
+        <v>30895</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>30010</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="3">
+        <v>32973</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{FFA0E461-2433-4EB9-90DA-E3A93FF638DE}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{CC2DAACF-F40E-41F0-805E-870694776725}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{39CE2935-ADD9-4488-8815-C1255C9E2B13}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{2D12770F-3E61-4E17-A3EC-5C62DCC55B54}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{BE22D71A-1DCA-429E-8B7E-0E3C5D350E28}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{4EF6C495-3D89-43C0-A7D2-CC42E4448A88}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{2588E24F-7896-4DB3-BFE1-654BA9962DB0}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{7DBFD881-AE99-4E22-9CB0-1131FA80EC46}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{975946E6-2716-40C0-93BF-2CE9DDCEE0F9}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{A458D354-003A-4E38-A3DB-27AF02B76310}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1110,18 +1944,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1139,32 +1973,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2065B93-80A0-4361-A2A5-7DD57587C3AE}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1177,46 +2011,255 @@
       <c r="A3">
         <v>190001</v>
       </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3">
+        <v>10001</v>
+      </c>
+      <c r="E3">
+        <v>200001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>190002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4">
+        <v>10001</v>
+      </c>
+      <c r="E4">
+        <v>200001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>190003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5">
+        <v>10001</v>
+      </c>
+      <c r="E5">
+        <v>200002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>190004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6">
+        <v>10001</v>
+      </c>
+      <c r="E6">
+        <v>200002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>190005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7">
+        <v>10001</v>
+      </c>
+      <c r="E7">
+        <v>200003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>190006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8">
+        <v>10001</v>
+      </c>
+      <c r="E8">
+        <v>200003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>190007</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9">
+        <v>10001</v>
+      </c>
+      <c r="E9">
+        <v>200004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>190008</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10">
+        <v>10001</v>
+      </c>
+      <c r="E10">
+        <v>200004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>190009</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11">
+        <v>10001</v>
+      </c>
+      <c r="E11">
+        <v>200005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>190010</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12">
+        <v>10001</v>
+      </c>
+      <c r="E12">
+        <v>200005</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6252F8EF-EEE5-4C58-9102-DEEEE939018F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>310001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>310002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>310003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>310004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>310005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>310006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1226,19 +2269,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73103244-3CE0-428D-8FF1-D2254FF786FD}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33:L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="133.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="13.88671875" customWidth="1"/>
@@ -1246,55 +2289,1717 @@
     <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" t="s">
-        <v>52</v>
-      </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>160001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>200002</v>
+      </c>
+      <c r="K3">
+        <v>190003</v>
+      </c>
+      <c r="L3">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>160002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>200002</v>
+      </c>
+      <c r="K4">
+        <v>190003</v>
+      </c>
+      <c r="L4">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>160003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>200002</v>
+      </c>
+      <c r="K5">
+        <v>190003</v>
+      </c>
+      <c r="L5">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>160004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>200002</v>
+      </c>
+      <c r="K6">
+        <v>190003</v>
+      </c>
+      <c r="L6">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>160005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>200002</v>
+      </c>
+      <c r="K7">
+        <v>190003</v>
+      </c>
+      <c r="L7">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>160006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>200002</v>
+      </c>
+      <c r="K8">
+        <v>190003</v>
+      </c>
+      <c r="L8">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>160007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>200002</v>
+      </c>
+      <c r="K9">
+        <v>190003</v>
+      </c>
+      <c r="L9">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>160008</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>58</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>200002</v>
+      </c>
+      <c r="K10">
+        <v>190003</v>
+      </c>
+      <c r="L10">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>160009</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11">
+        <v>89</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>200002</v>
+      </c>
+      <c r="K11">
+        <v>190004</v>
+      </c>
+      <c r="L11">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>160010</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>200002</v>
+      </c>
+      <c r="K12">
+        <v>190004</v>
+      </c>
+      <c r="L12">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>160011</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>200002</v>
+      </c>
+      <c r="K13">
+        <v>190004</v>
+      </c>
+      <c r="L13">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>160012</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>200002</v>
+      </c>
+      <c r="K14">
+        <v>190004</v>
+      </c>
+      <c r="L14">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>160013</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>200002</v>
+      </c>
+      <c r="K15">
+        <v>190004</v>
+      </c>
+      <c r="L15">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>160014</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16">
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>200002</v>
+      </c>
+      <c r="K16">
+        <v>190004</v>
+      </c>
+      <c r="L16">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>160015</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17">
+        <v>35</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17">
+        <v>34</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>200002</v>
+      </c>
+      <c r="K17">
+        <v>190004</v>
+      </c>
+      <c r="L17">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>160016</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>200002</v>
+      </c>
+      <c r="K18">
+        <v>190004</v>
+      </c>
+      <c r="L18">
+        <v>310005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>160017</v>
+      </c>
+      <c r="B19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>205</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>200005</v>
+      </c>
+      <c r="K19">
+        <v>190010</v>
+      </c>
+      <c r="L19">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>160018</v>
+      </c>
+      <c r="B20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>205</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>200005</v>
+      </c>
+      <c r="K20">
+        <v>190010</v>
+      </c>
+      <c r="L20">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>160019</v>
+      </c>
+      <c r="B21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>205</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>200005</v>
+      </c>
+      <c r="K21">
+        <v>190010</v>
+      </c>
+      <c r="L21">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>160020</v>
+      </c>
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E22">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>205</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>200005</v>
+      </c>
+      <c r="K22">
+        <v>190010</v>
+      </c>
+      <c r="L22">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>160021</v>
+      </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>200005</v>
+      </c>
+      <c r="K23">
+        <v>190010</v>
+      </c>
+      <c r="L23">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>160022</v>
+      </c>
+      <c r="B24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>205</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>200005</v>
+      </c>
+      <c r="K24">
+        <v>190010</v>
+      </c>
+      <c r="L24">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>160023</v>
+      </c>
+      <c r="B25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>205</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <v>200005</v>
+      </c>
+      <c r="K25">
+        <v>190010</v>
+      </c>
+      <c r="L25">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>160024</v>
+      </c>
+      <c r="B26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>205</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>200005</v>
+      </c>
+      <c r="K26">
+        <v>190010</v>
+      </c>
+      <c r="L26">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>160025</v>
+      </c>
+      <c r="B27" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27">
+        <v>13</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>200005</v>
+      </c>
+      <c r="K27">
+        <v>190010</v>
+      </c>
+      <c r="L27">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>160026</v>
+      </c>
+      <c r="B28" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E28">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>205</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>200005</v>
+      </c>
+      <c r="K28">
+        <v>190010</v>
+      </c>
+      <c r="L28">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>160027</v>
+      </c>
+      <c r="B29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E29">
+        <v>46</v>
+      </c>
+      <c r="F29" t="s">
+        <v>205</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>200005</v>
+      </c>
+      <c r="K29">
+        <v>190010</v>
+      </c>
+      <c r="L29">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>160028</v>
+      </c>
+      <c r="B30" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E30">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>205</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>200005</v>
+      </c>
+      <c r="K30">
+        <v>190010</v>
+      </c>
+      <c r="L30">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>160029</v>
+      </c>
+      <c r="B31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E31">
+        <v>48</v>
+      </c>
+      <c r="F31" t="s">
+        <v>205</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>200005</v>
+      </c>
+      <c r="K31">
+        <v>190010</v>
+      </c>
+      <c r="L31">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>160030</v>
+      </c>
+      <c r="B32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32">
+        <v>18</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E32">
+        <v>49</v>
+      </c>
+      <c r="F32" t="s">
+        <v>205</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>200005</v>
+      </c>
+      <c r="K32">
+        <v>190010</v>
+      </c>
+      <c r="L32">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>160031</v>
+      </c>
+      <c r="B33" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E33">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33">
+        <v>200005</v>
+      </c>
+      <c r="K33">
+        <v>190010</v>
+      </c>
+      <c r="L33">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>160032</v>
+      </c>
+      <c r="B34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>225</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>226</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>10</v>
+      </c>
+      <c r="J34">
+        <v>200005</v>
+      </c>
+      <c r="K34">
+        <v>190009</v>
+      </c>
+      <c r="L34">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>160033</v>
+      </c>
+      <c r="B35" t="s">
+        <v>210</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>225</v>
+      </c>
+      <c r="E35">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>226</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="J35">
+        <v>200005</v>
+      </c>
+      <c r="K35">
+        <v>190009</v>
+      </c>
+      <c r="L35">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>160034</v>
+      </c>
+      <c r="B36" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>226</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="J36">
+        <v>200005</v>
+      </c>
+      <c r="K36">
+        <v>190009</v>
+      </c>
+      <c r="L36">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>160035</v>
+      </c>
+      <c r="B37" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>225</v>
+      </c>
+      <c r="E37">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>226</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>10</v>
+      </c>
+      <c r="J37">
+        <v>200005</v>
+      </c>
+      <c r="K37">
+        <v>190009</v>
+      </c>
+      <c r="L37">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>160036</v>
+      </c>
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38">
+        <v>14</v>
+      </c>
+      <c r="F38" t="s">
+        <v>226</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>10</v>
+      </c>
+      <c r="J38">
+        <v>200005</v>
+      </c>
+      <c r="K38">
+        <v>190009</v>
+      </c>
+      <c r="L38">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>160037</v>
+      </c>
+      <c r="B39" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39">
+        <v>15</v>
+      </c>
+      <c r="F39" t="s">
+        <v>226</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <v>200005</v>
+      </c>
+      <c r="K39">
+        <v>190009</v>
+      </c>
+      <c r="L39">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>160038</v>
+      </c>
+      <c r="B40" t="s">
+        <v>215</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>226</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <v>200005</v>
+      </c>
+      <c r="K40">
+        <v>190009</v>
+      </c>
+      <c r="L40">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>160039</v>
+      </c>
+      <c r="B41" t="s">
+        <v>216</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>225</v>
+      </c>
+      <c r="E41">
+        <v>17</v>
+      </c>
+      <c r="F41" t="s">
+        <v>226</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>10</v>
+      </c>
+      <c r="J41">
+        <v>200005</v>
+      </c>
+      <c r="K41">
+        <v>190009</v>
+      </c>
+      <c r="L41">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>160040</v>
+      </c>
+      <c r="B42" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>226</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <v>200005</v>
+      </c>
+      <c r="K42">
+        <v>190009</v>
+      </c>
+      <c r="L42">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>160041</v>
+      </c>
+      <c r="B43" t="s">
+        <v>218</v>
+      </c>
+      <c r="C43">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>226</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="J43">
+        <v>200005</v>
+      </c>
+      <c r="K43">
+        <v>190009</v>
+      </c>
+      <c r="L43">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>160042</v>
+      </c>
+      <c r="B44" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>225</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>10</v>
+      </c>
+      <c r="J44">
+        <v>200005</v>
+      </c>
+      <c r="K44">
+        <v>190009</v>
+      </c>
+      <c r="L44">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>160043</v>
+      </c>
+      <c r="B45" t="s">
+        <v>220</v>
+      </c>
+      <c r="C45">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>225</v>
+      </c>
+      <c r="E45">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>226</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>10</v>
+      </c>
+      <c r="J45">
+        <v>200005</v>
+      </c>
+      <c r="K45">
+        <v>190009</v>
+      </c>
+      <c r="L45">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>160044</v>
+      </c>
+      <c r="B46" t="s">
+        <v>221</v>
+      </c>
+      <c r="C46">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>225</v>
+      </c>
+      <c r="E46">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>226</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="J46">
+        <v>200005</v>
+      </c>
+      <c r="K46">
+        <v>190009</v>
+      </c>
+      <c r="L46">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>160045</v>
+      </c>
+      <c r="B47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>225</v>
+      </c>
+      <c r="E47">
+        <v>23</v>
+      </c>
+      <c r="F47" t="s">
+        <v>226</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>10</v>
+      </c>
+      <c r="J47">
+        <v>200005</v>
+      </c>
+      <c r="K47">
+        <v>190009</v>
+      </c>
+      <c r="L47">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>160046</v>
+      </c>
+      <c r="B48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>225</v>
+      </c>
+      <c r="E48">
+        <v>24</v>
+      </c>
+      <c r="F48" t="s">
+        <v>226</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+      <c r="J48">
+        <v>200005</v>
+      </c>
+      <c r="K48">
+        <v>190009</v>
+      </c>
+      <c r="L48">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>160047</v>
+      </c>
+      <c r="B49" t="s">
+        <v>224</v>
+      </c>
+      <c r="C49">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>225</v>
+      </c>
+      <c r="E49">
+        <v>25</v>
+      </c>
+      <c r="F49" t="s">
+        <v>226</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>10</v>
+      </c>
+      <c r="J49">
+        <v>200005</v>
+      </c>
+      <c r="K49">
+        <v>190009</v>
+      </c>
+      <c r="L49">
+        <v>310006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>160048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>160049</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>160050</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>160051</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>160052</v>
       </c>
     </row>
   </sheetData>
@@ -1321,27 +4026,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>